<commit_message>
pdf printing and mom upload template update
</commit_message>
<xml_diff>
--- a/public/templates/MOM UPLOAD TEMPLATE.xlsx
+++ b/public/templates/MOM UPLOAD TEMPLATE.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jm.renon\Documents\2025\PROJECT-DOCS\mom-app\public\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A573950B-625E-42C7-A449-E3683D5ACCA9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBFF9D30-1262-440C-AFA7-B7A6DC72852B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="MoM Entries" sheetId="1" r:id="rId1"/>
+    <sheet name="TYPES" sheetId="2" state="hidden" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="26">
   <si>
     <t>CODE</t>
   </si>
@@ -61,6 +62,48 @@
   </si>
   <si>
     <t>AGENDA</t>
+  </si>
+  <si>
+    <t>End-month meeting</t>
+  </si>
+  <si>
+    <t>RDG 3+9 BR</t>
+  </si>
+  <si>
+    <t>ECOM 3+9 BR</t>
+  </si>
+  <si>
+    <t>MID MONTH MEETING</t>
+  </si>
+  <si>
+    <t>TMG ORIGINAL PLANS</t>
+  </si>
+  <si>
+    <t>HB CLEAN-UP DRIVE</t>
+  </si>
+  <si>
+    <t>JCB WITH TMG MEETING</t>
+  </si>
+  <si>
+    <t>BUSINESS REVIEW</t>
+  </si>
+  <si>
+    <t>BUDGET REVIEW - SCM</t>
+  </si>
+  <si>
+    <t>BUDGET REVIEW - RDG</t>
+  </si>
+  <si>
+    <t>EXPORT</t>
+  </si>
+  <si>
+    <t>SM</t>
+  </si>
+  <si>
+    <t>BUDGET REVIEW - TMG</t>
+  </si>
+  <si>
+    <t>EMAIL FROM JCB</t>
   </si>
 </sst>
 </file>
@@ -164,7 +207,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -202,6 +245,7 @@
     <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -485,7 +529,7 @@
   <dimension ref="A1:L116"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="E32" sqref="E32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -545,7 +589,9 @@
     <row r="2" spans="1:12">
       <c r="A2" s="1"/>
       <c r="B2" s="2"/>
-      <c r="C2" s="1"/>
+      <c r="C2" s="1" t="s">
+        <v>24</v>
+      </c>
       <c r="D2" s="1"/>
       <c r="E2" s="3"/>
       <c r="F2" s="3"/>
@@ -559,7 +605,9 @@
     <row r="3" spans="1:12">
       <c r="A3" s="1"/>
       <c r="B3" s="2"/>
-      <c r="C3" s="1"/>
+      <c r="C3" s="1" t="s">
+        <v>15</v>
+      </c>
       <c r="D3" s="1"/>
       <c r="E3" s="3"/>
       <c r="F3" s="3"/>
@@ -2154,5 +2202,106 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid Entry" error="Please select an option from the dropdown menu." promptTitle="Select Type" prompt="Please choose a type from the list_x000a_" xr:uid="{C21AEB33-4C35-4AA9-BF5E-F1DE4AC60CFD}">
+          <x14:formula1>
+            <xm:f>TYPES!$A:$A</xm:f>
+          </x14:formula1>
+          <xm:sqref>C1:C1048576</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{088BFC04-3B41-47BF-B2A9-9247070BBD5F}">
+  <dimension ref="A1:B14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C37" sqref="C37"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="22.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="15"/>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14" t="s">
+        <v>25</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>